<commit_message>
setlle null values on upload
</commit_message>
<xml_diff>
--- a/public/documents/shareholder_upload_template.xlsx
+++ b/public/documents/shareholder_upload_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\fmco\public\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E90FC51-8C72-4BD6-9EF5-A53122B79E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DBD25E-5A42-48E1-82A8-0AC6D59C6D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{5785B23F-EA69-420C-A0B0-16BE4589A641}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5785B23F-EA69-420C-A0B0-16BE4589A641}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Shareholder number</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Type (Individual/Institution)</t>
+  </si>
+  <si>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -461,11 +464,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A24E2BF-C28C-400E-A204-B0B611FE7005}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -479,10 +484,11 @@
     <col min="8" max="8" width="27" style="1" customWidth="1"/>
     <col min="9" max="9" width="24.90625" style="1" customWidth="1"/>
     <col min="10" max="10" width="24.1796875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="3"/>
+    <col min="11" max="11" width="28.54296875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,8 +519,11 @@
       <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B2" s="2"/>
     </row>
   </sheetData>

</xml_diff>